<commit_message>
ETMS changes and updated angular front end
</commit_message>
<xml_diff>
--- a/docs/ETMS Original Estimation.xlsx
+++ b/docs/ETMS Original Estimation.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EmployeeTimeManagementSystem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EmployeeTimeManagementSystem\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77D3437-11C2-41F0-B122-E3B297376CD8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBD11A8A-4EE9-42BA-8985-65299BECB019}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{75314B9F-328A-4DF2-A54B-A491B946C939}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="65">
   <si>
     <t>Employee Time Management System</t>
   </si>
@@ -220,6 +220,12 @@
   </si>
   <si>
     <t>Final all feature Integration Testing &amp; Bug fixing</t>
+  </si>
+  <si>
+    <t>remaining</t>
+  </si>
+  <si>
+    <t>completed</t>
   </si>
 </sst>
 </file>
@@ -810,8 +816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{129B7D34-8229-4C47-B000-384C739276FB}">
   <dimension ref="A1:E98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -819,7 +825,8 @@
     <col min="1" max="1" width="8.88671875" style="15"/>
     <col min="2" max="2" width="70.6640625" style="2" customWidth="1"/>
     <col min="3" max="3" width="22" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="2"/>
+    <col min="4" max="4" width="10.5546875" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.35">
@@ -841,8 +848,12 @@
       <c r="C2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="D2" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
@@ -861,6 +872,12 @@
       <c r="C4" s="13">
         <v>3</v>
       </c>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="12">
@@ -870,6 +887,12 @@
         <v>3</v>
       </c>
       <c r="C5" s="13">
+        <v>3</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
         <v>3</v>
       </c>
     </row>
@@ -883,6 +906,12 @@
       <c r="C6" s="13">
         <v>3</v>
       </c>
+      <c r="D6" s="2">
+        <v>2</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
@@ -893,6 +922,12 @@
       </c>
       <c r="C7" s="13">
         <v>3</v>
+      </c>
+      <c r="D7" s="2">
+        <v>3</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -922,6 +957,9 @@
       <c r="C11" s="13">
         <v>2</v>
       </c>
+      <c r="D11" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="12"/>
@@ -947,6 +985,9 @@
       <c r="C14" s="13">
         <v>1</v>
       </c>
+      <c r="D14" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="12"/>
@@ -956,6 +997,9 @@
       <c r="C15" s="13">
         <v>2</v>
       </c>
+      <c r="D15" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="12"/>
@@ -965,8 +1009,11 @@
       <c r="C16" s="13">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E16" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="12">
         <v>7</v>
       </c>
@@ -975,7 +1022,7 @@
       </c>
       <c r="C17" s="13"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="12"/>
       <c r="B18" s="5" t="s">
         <v>13</v>
@@ -983,8 +1030,11 @@
       <c r="C18" s="13">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E18" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="12"/>
       <c r="B19" s="5" t="s">
         <v>15</v>
@@ -992,8 +1042,11 @@
       <c r="C19" s="13">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E19" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="12"/>
       <c r="B20" s="5" t="s">
         <v>17</v>
@@ -1001,8 +1054,11 @@
       <c r="C20" s="13">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E20" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="12">
         <v>8</v>
       </c>
@@ -1011,7 +1067,7 @@
       </c>
       <c r="C21" s="13"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="12"/>
       <c r="B22" s="5" t="s">
         <v>13</v>
@@ -1019,8 +1075,11 @@
       <c r="C22" s="13">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E22" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="12"/>
       <c r="B23" s="5" t="s">
         <v>15</v>
@@ -1028,8 +1087,11 @@
       <c r="C23" s="13">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E23" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="12"/>
       <c r="B24" s="5" t="s">
         <v>17</v>
@@ -1037,15 +1099,18 @@
       <c r="C24" s="13">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E24" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="12"/>
       <c r="B25" s="19" t="s">
         <v>18</v>
       </c>
       <c r="C25" s="13"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="12">
         <v>9</v>
       </c>
@@ -1054,7 +1119,7 @@
       </c>
       <c r="C26" s="13"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="12"/>
       <c r="B27" s="5" t="s">
         <v>20</v>
@@ -1062,8 +1127,11 @@
       <c r="C27" s="13">
         <v>3</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D27" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="12"/>
       <c r="B28" s="5" t="s">
         <v>19</v>
@@ -1071,8 +1139,14 @@
       <c r="C28" s="13">
         <v>4</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D28" s="2">
+        <v>2</v>
+      </c>
+      <c r="E28" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="12"/>
       <c r="B29" s="5" t="s">
         <v>17</v>
@@ -1081,7 +1155,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="12">
         <v>10</v>
       </c>
@@ -1090,7 +1164,7 @@
       </c>
       <c r="C30" s="13"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="12"/>
       <c r="B31" s="5" t="s">
         <v>13</v>
@@ -1098,8 +1172,11 @@
       <c r="C31" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D31" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="12"/>
       <c r="B32" s="5" t="s">
         <v>22</v>
@@ -1107,8 +1184,14 @@
       <c r="C32" s="13">
         <v>3</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D32" s="2">
+        <v>2</v>
+      </c>
+      <c r="E32" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="12"/>
       <c r="B33" s="5" t="s">
         <v>17</v>
@@ -1117,7 +1200,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="12">
         <v>11</v>
       </c>
@@ -1126,7 +1209,7 @@
       </c>
       <c r="C34" s="13"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="12"/>
       <c r="B35" s="5" t="s">
         <v>13</v>
@@ -1134,8 +1217,11 @@
       <c r="C35" s="13">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E35" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="12"/>
       <c r="B36" s="5" t="s">
         <v>15</v>
@@ -1143,8 +1229,11 @@
       <c r="C36" s="13">
         <v>2</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E36" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="12"/>
       <c r="B37" s="5" t="s">
         <v>17</v>
@@ -1152,8 +1241,11 @@
       <c r="C37" s="13">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E37" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="12">
         <v>12</v>
       </c>
@@ -1162,7 +1254,7 @@
       </c>
       <c r="C38" s="13"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="12"/>
       <c r="B39" s="5" t="s">
         <v>25</v>
@@ -1170,8 +1262,11 @@
       <c r="C39" s="13">
         <v>3</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E39" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="12"/>
       <c r="B40" s="5" t="s">
         <v>26</v>
@@ -1179,8 +1274,11 @@
       <c r="C40" s="13">
         <v>3</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E40" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="12"/>
       <c r="B41" s="5" t="s">
         <v>17</v>
@@ -1188,15 +1286,18 @@
       <c r="C41" s="13">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E41" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="12"/>
       <c r="B42" s="19" t="s">
         <v>27</v>
       </c>
       <c r="C42" s="13"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="12">
         <v>10</v>
       </c>
@@ -1205,7 +1306,7 @@
       </c>
       <c r="C43" s="13"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="12"/>
       <c r="B44" s="5" t="s">
         <v>30</v>
@@ -1213,8 +1314,14 @@
       <c r="C44" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D44" s="2">
+        <v>0</v>
+      </c>
+      <c r="E44" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="12"/>
       <c r="B45" s="5" t="s">
         <v>31</v>
@@ -1222,8 +1329,14 @@
       <c r="C45" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D45" s="2">
+        <v>0</v>
+      </c>
+      <c r="E45" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="12"/>
       <c r="B46" s="5" t="s">
         <v>17</v>
@@ -1231,8 +1344,11 @@
       <c r="C46" s="13">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E46" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="12">
         <v>11</v>
       </c>
@@ -1241,7 +1357,7 @@
       </c>
       <c r="C47" s="13"/>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="12"/>
       <c r="B48" s="5" t="s">
         <v>13</v>
@@ -1249,8 +1365,11 @@
       <c r="C48" s="13">
         <v>2</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D48" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="12"/>
       <c r="B49" s="5" t="s">
         <v>33</v>
@@ -1258,8 +1377,11 @@
       <c r="C49" s="13">
         <v>2</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D49" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="12"/>
       <c r="B50" s="5" t="s">
         <v>17</v>
@@ -1267,8 +1389,11 @@
       <c r="C50" s="13">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E50" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="12">
         <v>12</v>
       </c>
@@ -1277,7 +1402,7 @@
       </c>
       <c r="C51" s="13"/>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="12"/>
       <c r="B52" s="5" t="s">
         <v>13</v>
@@ -1285,8 +1410,14 @@
       <c r="C52" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D52" s="2">
+        <v>1</v>
+      </c>
+      <c r="E52" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="12"/>
       <c r="B53" s="5" t="s">
         <v>15</v>
@@ -1294,8 +1425,14 @@
       <c r="C53" s="13">
         <v>2</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D53" s="2">
+        <v>1</v>
+      </c>
+      <c r="E53" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="12"/>
       <c r="B54" s="5" t="s">
         <v>17</v>
@@ -1303,8 +1440,11 @@
       <c r="C54" s="13">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E54" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="12">
         <v>13</v>
       </c>
@@ -1313,7 +1453,7 @@
       </c>
       <c r="C55" s="13"/>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="12"/>
       <c r="B56" s="5" t="s">
         <v>13</v>
@@ -1321,8 +1461,14 @@
       <c r="C56" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D56" s="2">
+        <v>1</v>
+      </c>
+      <c r="E56" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="12"/>
       <c r="B57" s="5" t="s">
         <v>36</v>
@@ -1330,8 +1476,14 @@
       <c r="C57" s="13">
         <v>2</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D57" s="2">
+        <v>1</v>
+      </c>
+      <c r="E57" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="12"/>
       <c r="B58" s="5" t="s">
         <v>17</v>
@@ -1339,8 +1491,11 @@
       <c r="C58" s="13">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E58" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="12">
         <v>14</v>
       </c>
@@ -1349,7 +1504,7 @@
       </c>
       <c r="C59" s="13"/>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="12"/>
       <c r="B60" s="5" t="s">
         <v>13</v>
@@ -1357,8 +1512,14 @@
       <c r="C60" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D60" s="2">
+        <v>0</v>
+      </c>
+      <c r="E60" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="12"/>
       <c r="B61" s="5" t="s">
         <v>15</v>
@@ -1366,8 +1527,14 @@
       <c r="C61" s="13">
         <v>2</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D61" s="2">
+        <v>0</v>
+      </c>
+      <c r="E61" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="12"/>
       <c r="B62" s="5" t="s">
         <v>17</v>
@@ -1375,8 +1542,14 @@
       <c r="C62" s="13">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D62" s="2">
+        <v>0</v>
+      </c>
+      <c r="E62" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="12">
         <v>15</v>
       </c>
@@ -1385,7 +1558,7 @@
       </c>
       <c r="C63" s="13"/>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="12"/>
       <c r="B64" s="5" t="s">
         <v>39</v>
@@ -1393,8 +1566,14 @@
       <c r="C64" s="13">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D64" s="2">
+        <v>0</v>
+      </c>
+      <c r="E64" s="2">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="12"/>
       <c r="B65" s="5" t="s">
         <v>40</v>
@@ -1402,8 +1581,14 @@
       <c r="C65" s="13">
         <v>4</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D65" s="2">
+        <v>0</v>
+      </c>
+      <c r="E65" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="12"/>
       <c r="B66" s="5" t="s">
         <v>17</v>
@@ -1411,8 +1596,14 @@
       <c r="C66" s="13">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D66" s="2">
+        <v>0</v>
+      </c>
+      <c r="E66" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="12">
         <v>16</v>
       </c>
@@ -1421,7 +1612,7 @@
       </c>
       <c r="C67" s="13"/>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="12"/>
       <c r="B68" s="5" t="s">
         <v>13</v>
@@ -1429,8 +1620,14 @@
       <c r="C68" s="13">
         <v>2</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D68" s="2">
+        <v>0</v>
+      </c>
+      <c r="E68" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="12"/>
       <c r="B69" s="5" t="s">
         <v>36</v>
@@ -1438,8 +1635,14 @@
       <c r="C69" s="13">
         <v>2</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D69" s="2">
+        <v>0</v>
+      </c>
+      <c r="E69" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="12"/>
       <c r="B70" s="5" t="s">
         <v>17</v>
@@ -1447,20 +1650,26 @@
       <c r="C70" s="13">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D70" s="2">
+        <v>0</v>
+      </c>
+      <c r="E70" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="12"/>
       <c r="B71" s="5"/>
       <c r="C71" s="13"/>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="16"/>
       <c r="B72" s="18" t="s">
         <v>53</v>
       </c>
       <c r="C72" s="17"/>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="12">
         <v>17</v>
       </c>
@@ -1469,7 +1678,7 @@
       </c>
       <c r="C73" s="13"/>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="12"/>
       <c r="B74" s="5" t="s">
         <v>43</v>
@@ -1477,8 +1686,14 @@
       <c r="C74" s="13">
         <v>2</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D74" s="2">
+        <v>1</v>
+      </c>
+      <c r="E74" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="12"/>
       <c r="B75" s="5" t="s">
         <v>17</v>
@@ -1486,8 +1701,14 @@
       <c r="C75" s="13">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D75" s="2">
+        <v>0</v>
+      </c>
+      <c r="E75" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="12">
         <v>18</v>
       </c>
@@ -1496,7 +1717,7 @@
       </c>
       <c r="C76" s="13"/>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="12"/>
       <c r="B77" s="5" t="s">
         <v>45</v>
@@ -1504,8 +1725,14 @@
       <c r="C77" s="13">
         <v>2</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D77" s="2">
+        <v>2</v>
+      </c>
+      <c r="E77" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="12"/>
       <c r="B78" s="5" t="s">
         <v>17</v>
@@ -1513,8 +1740,14 @@
       <c r="C78" s="13">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D78" s="2">
+        <v>0</v>
+      </c>
+      <c r="E78" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="12">
         <v>19</v>
       </c>
@@ -1523,7 +1756,7 @@
       </c>
       <c r="C79" s="13"/>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" s="12"/>
       <c r="B80" s="5" t="s">
         <v>47</v>
@@ -1531,8 +1764,14 @@
       <c r="C80" s="13">
         <v>2</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D80" s="2">
+        <v>2</v>
+      </c>
+      <c r="E80" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="12"/>
       <c r="B81" s="5" t="s">
         <v>17</v>
@@ -1540,8 +1779,14 @@
       <c r="C81" s="13">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D81" s="2">
+        <v>0</v>
+      </c>
+      <c r="E81" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" s="12">
         <v>20</v>
       </c>
@@ -1550,7 +1795,7 @@
       </c>
       <c r="C82" s="13"/>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" s="12"/>
       <c r="B83" s="5" t="s">
         <v>57</v>
@@ -1558,8 +1803,14 @@
       <c r="C83" s="13">
         <v>2</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D83" s="2">
+        <v>1</v>
+      </c>
+      <c r="E83" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" s="12"/>
       <c r="B84" s="5" t="s">
         <v>17</v>
@@ -1567,8 +1818,14 @@
       <c r="C84" s="13">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D84" s="2">
+        <v>0</v>
+      </c>
+      <c r="E84" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" s="12">
         <v>21</v>
       </c>
@@ -1577,7 +1834,7 @@
       </c>
       <c r="C85" s="13"/>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" s="12"/>
       <c r="B86" s="5" t="s">
         <v>54</v>
@@ -1585,8 +1842,14 @@
       <c r="C86" s="13">
         <v>2</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D86" s="2">
+        <v>0</v>
+      </c>
+      <c r="E86" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" s="12"/>
       <c r="B87" s="5" t="s">
         <v>17</v>
@@ -1594,8 +1857,14 @@
       <c r="C87" s="13">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D87" s="2">
+        <v>0</v>
+      </c>
+      <c r="E87" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" s="12">
         <v>22</v>
       </c>
@@ -1605,8 +1874,14 @@
       <c r="C88" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D88" s="2">
+        <v>2</v>
+      </c>
+      <c r="E88" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" s="12">
         <v>23</v>
       </c>
@@ -1616,20 +1891,26 @@
       <c r="C89" s="13">
         <v>2</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D89" s="2">
+        <v>2</v>
+      </c>
+      <c r="E89" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" s="12"/>
       <c r="B90" s="5"/>
       <c r="C90" s="13"/>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" s="16"/>
       <c r="B91" s="18" t="s">
         <v>58</v>
       </c>
       <c r="C91" s="17"/>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" s="12">
         <v>24</v>
       </c>
@@ -1639,8 +1920,14 @@
       <c r="C92" s="13">
         <v>5</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D92" s="2">
+        <v>0</v>
+      </c>
+      <c r="E92" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" s="12">
         <v>25</v>
       </c>
@@ -1650,13 +1937,19 @@
       <c r="C93" s="13">
         <v>2</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D93" s="2">
+        <v>2</v>
+      </c>
+      <c r="E93" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" s="12"/>
       <c r="B94" s="5"/>
       <c r="C94" s="13"/>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" s="12"/>
       <c r="B95" s="4" t="s">
         <v>51</v>
@@ -1665,8 +1958,16 @@
         <f>SUM(C4:C93)</f>
         <v>96</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D95" s="2">
+        <f>SUM(D4:D94)</f>
+        <v>38</v>
+      </c>
+      <c r="E95" s="2">
+        <f>SUM(E4:E94)</f>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" s="12"/>
       <c r="B96" s="4" t="s">
         <v>55</v>

</xml_diff>